<commit_message>
Organização e plotagem de gráficos
</commit_message>
<xml_diff>
--- a/Projeto_2_cdados.xlsx
+++ b/Projeto_2_cdados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Projeto-2-Cdados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8ddea9f9bcd6aca2/Documentos/2º Semestre/Ciência dos Dados/Projeto 2/Projeto-2-Cdados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8A5BC2-D04A-41BC-AA07-BDA972CD2261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5DAEAF9B-DA76-4F90-BD88-C6CCEAC67928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{380501EF-B0C2-4CE2-B4D4-5742166DC9A6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="30">
   <si>
     <t>Idade</t>
   </si>
@@ -79,332 +79,44 @@
     <t>De 1 a 3 horas</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
-    <t>6 horas</t>
-  </si>
-  <si>
-    <t>5 horas</t>
-  </si>
-  <si>
-    <t>3 a 4 horas</t>
-  </si>
-  <si>
     <t>Estudante de colegial</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 horas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 a 2 horas </t>
-  </si>
-  <si>
-    <t>4 horas</t>
-  </si>
-  <si>
-    <t>4-5 horas</t>
   </si>
   <si>
     <t>Menos de 1 hora</t>
   </si>
   <si>
-    <t>Uma hora</t>
-  </si>
-  <si>
-    <t>6 horas pelo menos</t>
-  </si>
-  <si>
     <t>Sim, diminui o número de horas</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t>agora meu trabalho é todo online em vez de presencial então aumentou mas só nos dias que eu trabalho</t>
-  </si>
-  <si>
-    <t>Mais do que devia</t>
-  </si>
-  <si>
-    <t>De 3 a 5 horas</t>
-  </si>
-  <si>
-    <t>Antes era entre 4 e 6 horas, agora é entre 7 e 10 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 a 5 horas </t>
-  </si>
-  <si>
-    <t>2 horas diarias</t>
-  </si>
-  <si>
-    <t>2 a 3 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">em media 8 hrs </t>
-  </si>
-  <si>
-    <t>2 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mais de 4hrs com certeza </t>
-  </si>
-  <si>
-    <t>3 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">na época de ead 8h ou mais, agr está voltando </t>
-  </si>
-  <si>
-    <t>5 horas, talvez</t>
-  </si>
-  <si>
-    <t>quase o número total de horas que eu fico hoje em dia, já que passava o dia na escola e agora estou em ead.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6h </t>
-  </si>
-  <si>
-    <t>Cerca de 5 horas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 horas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cerca de 8 hr </t>
-  </si>
-  <si>
-    <t>15h</t>
-  </si>
-  <si>
-    <t>Por volta de 3horas</t>
-  </si>
-  <si>
-    <t>Acho que umas 4....ou 10 kkkkk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aumento em duas horas </t>
-  </si>
-  <si>
-    <t>Acho que certa de quatro horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+2h mais ou menos </t>
-  </si>
-  <si>
-    <t>10 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 a 6 horas </t>
-  </si>
-  <si>
-    <t>Duas horas.</t>
-  </si>
-  <si>
-    <t>± 7</t>
-  </si>
-  <si>
-    <t>1hr ou 1:30hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 horas </t>
-  </si>
-  <si>
-    <t>De 3 a 7 horas por dia.</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>3horas</t>
-  </si>
-  <si>
-    <t>Na época de EaD umas 10 horas ou mais.</t>
-  </si>
-  <si>
-    <t>Não sei kkkk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 horas </t>
-  </si>
-  <si>
-    <t>1h/2h</t>
-  </si>
-  <si>
-    <t>Umas 3h</t>
-  </si>
-  <si>
-    <t>muito mais</t>
-  </si>
-  <si>
-    <t>5h mais ou menos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-4 horas </t>
-  </si>
-  <si>
-    <t>4 a 5</t>
-  </si>
-  <si>
-    <t>aumaumentou umas 5horas</t>
-  </si>
-  <si>
-    <t>De uma à duas horas.</t>
-  </si>
-  <si>
-    <t>4 horas a mais pir causa do ead</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>3hrs</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>umas 3hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aumentei de no máximo 6 horas par no mínimo 8 horas por dia </t>
-  </si>
-  <si>
-    <t>SLA, umas 5</t>
-  </si>
-  <si>
-    <t>Várias. Sério, antes eu nem usava computador direito, hoje em dia passo o dia nele jogando e fazendo trabalhos da escola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Umas 5 horas a mais </t>
-  </si>
-  <si>
-    <t>Devido às aulas on-line, devo ter aumentado o meu tempo conectada em 5 horas</t>
-  </si>
-  <si>
-    <t>Mais de duas horas por dia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-3 horas </t>
-  </si>
-  <si>
-    <t>4-5</t>
-  </si>
-  <si>
-    <t>1h30min</t>
-  </si>
-  <si>
-    <t>Mais de 5 horas</t>
-  </si>
-  <si>
-    <t>8 horas</t>
-  </si>
-  <si>
-    <t>2 a 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aproximadamente 3 horas </t>
-  </si>
-  <si>
-    <t>1 ou 2</t>
-  </si>
-  <si>
-    <t>10hrs</t>
-  </si>
-  <si>
-    <t>3 hrs</t>
-  </si>
-  <si>
-    <t>Mais de 12 horas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5h </t>
-  </si>
-  <si>
-    <t>1 hora</t>
-  </si>
-  <si>
-    <t>umas 3 horas, acho</t>
-  </si>
-  <si>
-    <t>não faço ideia</t>
-  </si>
-  <si>
-    <t>Acredito que umas 3 à 4 horas.</t>
-  </si>
-  <si>
-    <t>Acho que umas 2 horas, principalmente na época do ead, mas já que voltamos com as presenciais, acredito ter normalizado mais um pouco.</t>
-  </si>
-  <si>
-    <t>dobrado</t>
-  </si>
-  <si>
-    <t>3/4</t>
-  </si>
-  <si>
-    <t>não aumentou</t>
-  </si>
-  <si>
-    <t>Não aumentou</t>
-  </si>
-  <si>
-    <t>4horas</t>
-  </si>
-  <si>
-    <t>7 horas</t>
-  </si>
-  <si>
-    <t>8h</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2h</t>
-  </si>
-  <si>
-    <t>5h</t>
-  </si>
-  <si>
-    <t>1 hrs</t>
-  </si>
-  <si>
-    <t>9 horas</t>
-  </si>
-  <si>
-    <t>4hrs</t>
   </si>
   <si>
     <t>Estado</t>
   </si>
   <si>
-    <t>Diaria</t>
+    <t>Horas</t>
   </si>
   <si>
-    <t>Vontade</t>
+    <t>Pandemia</t>
   </si>
   <si>
     <t>Aumento</t>
   </si>
   <si>
-    <t>Retomando</t>
+    <t>Retomada</t>
   </si>
   <si>
     <t>Ajuda</t>
   </si>
   <si>
-    <t>Media</t>
+    <t>Emprego</t>
   </si>
   <si>
-    <t>Emprego</t>
+    <t>Vontade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -418,6 +130,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -442,12 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -667,11 +387,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J194"/>
+  <dimension ref="A1:J195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -684,7 +404,7 @@
     <col min="9" max="17" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,31 +412,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>125</v>
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>18</v>
       </c>
@@ -736,10 +456,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
@@ -748,9 +468,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -770,8 +490,8 @@
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>101</v>
+      <c r="H3" s="2">
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
@@ -780,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>19</v>
       </c>
@@ -802,8 +522,8 @@
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>42</v>
+      <c r="H4" s="2">
+        <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
@@ -812,14 +532,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -834,8 +554,8 @@
       <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>110</v>
+      <c r="H5" s="2">
+        <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>11</v>
@@ -844,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>48</v>
       </c>
@@ -866,8 +586,8 @@
       <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
+      <c r="H6" s="2">
+        <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>11</v>
@@ -876,7 +596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>19</v>
       </c>
@@ -898,8 +618,8 @@
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>44</v>
+      <c r="H7" s="2">
+        <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>11</v>
@@ -908,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>56</v>
       </c>
@@ -930,8 +650,8 @@
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>101</v>
+      <c r="H8" s="2">
+        <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>6</v>
@@ -940,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -962,8 +682,8 @@
       <c r="G9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>117</v>
+      <c r="H9" s="2">
+        <v>4</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>6</v>
@@ -972,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>19</v>
       </c>
@@ -1004,7 +724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>19</v>
       </c>
@@ -1026,8 +746,8 @@
       <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
+      <c r="H11" s="2">
+        <v>3</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>6</v>
@@ -1036,7 +756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>19</v>
       </c>
@@ -1058,8 +778,8 @@
       <c r="G12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>116</v>
+      <c r="H12" s="2">
+        <v>9</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>11</v>
@@ -1068,7 +788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>19</v>
       </c>
@@ -1090,8 +810,8 @@
       <c r="G13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>115</v>
+      <c r="H13" s="2">
+        <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>11</v>
@@ -1100,7 +820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>18</v>
       </c>
@@ -1122,8 +842,8 @@
       <c r="G14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>42</v>
+      <c r="H14" s="2">
+        <v>2</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>11</v>
@@ -1132,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>19</v>
       </c>
@@ -1154,8 +874,8 @@
       <c r="G15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>44</v>
+      <c r="H15" s="2">
+        <v>3</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>6</v>
@@ -1164,7 +884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>19</v>
       </c>
@@ -1186,8 +906,8 @@
       <c r="G16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>97</v>
+      <c r="H16" s="2">
+        <v>10</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>11</v>
@@ -1196,7 +916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>20</v>
       </c>
@@ -1218,8 +938,8 @@
       <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>42</v>
+      <c r="H17" s="2">
+        <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>6</v>
@@ -1228,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>19</v>
       </c>
@@ -1260,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>63</v>
       </c>
@@ -1282,8 +1002,8 @@
       <c r="G19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>19</v>
+      <c r="H19" s="2">
+        <v>3</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>11</v>
@@ -1292,7 +1012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>34</v>
       </c>
@@ -1314,8 +1034,8 @@
       <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>108</v>
+      <c r="H20" s="2">
+        <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>11</v>
@@ -1324,7 +1044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1346,8 +1066,8 @@
       <c r="G21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>20</v>
+      <c r="H21" s="2">
+        <v>6</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>9</v>
@@ -1356,7 +1076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -1378,8 +1098,8 @@
       <c r="G22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>21</v>
+      <c r="H22" s="2">
+        <v>5</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>11</v>
@@ -1388,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>50</v>
       </c>
@@ -1420,7 +1140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1442,8 +1162,8 @@
       <c r="G24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>22</v>
+      <c r="H24" s="2">
+        <v>4</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>9</v>
@@ -1452,7 +1172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>57</v>
       </c>
@@ -1484,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>17</v>
       </c>
@@ -1495,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>16</v>
@@ -1516,7 +1236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>20</v>
       </c>
@@ -1538,8 +1258,8 @@
       <c r="G27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>24</v>
+      <c r="H27" s="2">
+        <v>4</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>9</v>
@@ -1548,7 +1268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>20</v>
       </c>
@@ -1570,8 +1290,8 @@
       <c r="G28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>25</v>
+      <c r="H28" s="2">
+        <v>3</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>11</v>
@@ -1580,7 +1300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>19</v>
       </c>
@@ -1612,7 +1332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>25</v>
       </c>
@@ -1634,8 +1354,8 @@
       <c r="G30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>26</v>
+      <c r="H30" s="2">
+        <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>11</v>
@@ -1644,7 +1364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>57</v>
       </c>
@@ -1666,8 +1386,8 @@
       <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>25</v>
+      <c r="H31" s="2">
+        <v>3</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>11</v>
@@ -1676,7 +1396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>19</v>
       </c>
@@ -1698,8 +1418,8 @@
       <c r="G32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>27</v>
+      <c r="H32" s="2">
+        <v>4</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>6</v>
@@ -1708,7 +1428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>20</v>
       </c>
@@ -1740,7 +1460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>18</v>
       </c>
@@ -1762,8 +1482,8 @@
       <c r="G34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>28</v>
+      <c r="H34" s="2">
+        <v>4</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>11</v>
@@ -1772,7 +1492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>19</v>
       </c>
@@ -1794,8 +1514,8 @@
       <c r="G35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>108</v>
+      <c r="H35" s="2">
+        <v>0</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>11</v>
@@ -1804,7 +1524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>18</v>
       </c>
@@ -1836,7 +1556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>53</v>
       </c>
@@ -1868,7 +1588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>19</v>
       </c>
@@ -1900,7 +1620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>56</v>
       </c>
@@ -1914,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>9</v>
@@ -1922,8 +1642,8 @@
       <c r="G39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>30</v>
+      <c r="H39" s="2">
+        <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>6</v>
@@ -1932,7 +1652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>19</v>
       </c>
@@ -1954,8 +1674,8 @@
       <c r="G40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>31</v>
+      <c r="H40" s="2">
+        <v>6</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>6</v>
@@ -1964,7 +1684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>20</v>
       </c>
@@ -1996,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>20</v>
       </c>
@@ -2018,6 +1738,9 @@
       <c r="G42" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H42" s="2">
+        <v>3</v>
+      </c>
       <c r="I42" s="2" t="s">
         <v>6</v>
       </c>
@@ -2025,7 +1748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>21</v>
       </c>
@@ -2057,7 +1780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>19</v>
       </c>
@@ -2077,10 +1800,10 @@
         <v>6</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>93</v>
+        <v>21</v>
+      </c>
+      <c r="H44" s="2">
+        <v>8</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>11</v>
@@ -2089,7 +1812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>19</v>
       </c>
@@ -2111,8 +1834,8 @@
       <c r="G45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>33</v>
+      <c r="H45" s="3">
+        <v>3</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>6</v>
@@ -2121,7 +1844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>21</v>
       </c>
@@ -2143,8 +1866,8 @@
       <c r="G46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>34</v>
+      <c r="H46" s="2">
+        <v>6</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>11</v>
@@ -2153,7 +1876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>19</v>
       </c>
@@ -2175,8 +1898,8 @@
       <c r="G47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>35</v>
+      <c r="H47" s="2">
+        <v>10</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>9</v>
@@ -2185,7 +1908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>19</v>
       </c>
@@ -2207,8 +1930,8 @@
       <c r="G48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>36</v>
+      <c r="H48" s="2">
+        <v>5</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>11</v>
@@ -2217,7 +1940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>18</v>
       </c>
@@ -2239,8 +1962,8 @@
       <c r="G49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>108</v>
+      <c r="H49" s="2">
+        <v>0</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>6</v>
@@ -2249,7 +1972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>19</v>
       </c>
@@ -2271,8 +1994,8 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>37</v>
+      <c r="H50" s="2">
+        <v>3</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>11</v>
@@ -2281,7 +2004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>23</v>
       </c>
@@ -2303,8 +2026,8 @@
       <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>24</v>
+      <c r="H51" s="2">
+        <v>4</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>6</v>
@@ -2313,7 +2036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>20</v>
       </c>
@@ -2345,7 +2068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>19</v>
       </c>
@@ -2367,8 +2090,8 @@
       <c r="G53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="2" t="s">
-        <v>38</v>
+      <c r="H53" s="2">
+        <v>5</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>11</v>
@@ -2377,7 +2100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>18</v>
       </c>
@@ -2409,7 +2132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>19</v>
       </c>
@@ -2431,8 +2154,8 @@
       <c r="G55" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>39</v>
+      <c r="H55" s="2">
+        <v>2</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>11</v>
@@ -2441,7 +2164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>23</v>
       </c>
@@ -2463,8 +2186,8 @@
       <c r="G56" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>109</v>
+      <c r="H56" s="2">
+        <v>0</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>6</v>
@@ -2473,7 +2196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>18</v>
       </c>
@@ -2505,7 +2228,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>18</v>
       </c>
@@ -2516,7 +2239,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>16</v>
@@ -2527,8 +2250,8 @@
       <c r="G58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>40</v>
+      <c r="H58" s="2">
+        <v>3</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>6</v>
@@ -2537,7 +2260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>18</v>
       </c>
@@ -2559,8 +2282,8 @@
       <c r="G59" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H59" s="2" t="s">
-        <v>41</v>
+      <c r="H59" s="2">
+        <v>8</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>9</v>
@@ -2569,7 +2292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>19</v>
       </c>
@@ -2591,8 +2314,8 @@
       <c r="G60" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>42</v>
+      <c r="H60" s="2">
+        <v>2</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>11</v>
@@ -2601,7 +2324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>18</v>
       </c>
@@ -2623,8 +2346,8 @@
       <c r="G61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>43</v>
+      <c r="H61" s="2">
+        <v>4</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>6</v>
@@ -2633,7 +2356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>20</v>
       </c>
@@ -2655,8 +2378,8 @@
       <c r="G62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>44</v>
+      <c r="H62" s="2">
+        <v>3</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>6</v>
@@ -2665,7 +2388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>17</v>
       </c>
@@ -2676,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>16</v>
@@ -2687,8 +2410,8 @@
       <c r="G63" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>45</v>
+      <c r="H63" s="2">
+        <v>8</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>6</v>
@@ -2697,7 +2420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>17</v>
       </c>
@@ -2729,7 +2452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>17</v>
       </c>
@@ -2740,7 +2463,7 @@
         <v>14</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>18</v>
@@ -2751,6 +2474,9 @@
       <c r="G65" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H65" s="2">
+        <v>2</v>
+      </c>
       <c r="I65" s="2" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>18</v>
       </c>
@@ -2780,8 +2506,8 @@
       <c r="G66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="2" t="s">
-        <v>46</v>
+      <c r="H66" s="2">
+        <v>5</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>6</v>
@@ -2790,7 +2516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>19</v>
       </c>
@@ -2812,8 +2538,8 @@
       <c r="G67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>19</v>
+      <c r="H67" s="2">
+        <v>3</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>9</v>
@@ -2822,7 +2548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>15</v>
       </c>
@@ -2833,7 +2559,7 @@
         <v>3</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>5</v>
@@ -2844,8 +2570,8 @@
       <c r="G68" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>47</v>
+      <c r="H68" s="2">
+        <v>13</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>9</v>
@@ -2854,7 +2580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>18</v>
       </c>
@@ -2865,7 +2591,7 @@
         <v>3</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>8</v>
@@ -2886,7 +2612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>17</v>
       </c>
@@ -2897,7 +2623,7 @@
         <v>3</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>8</v>
@@ -2908,8 +2634,8 @@
       <c r="G70" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="2" t="s">
-        <v>48</v>
+      <c r="H70" s="2">
+        <v>6</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>6</v>
@@ -2918,7 +2644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>18</v>
       </c>
@@ -2950,7 +2676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>17</v>
       </c>
@@ -2961,7 +2687,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>5</v>
@@ -2972,8 +2698,8 @@
       <c r="G72" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>49</v>
+      <c r="H72" s="2">
+        <v>5</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>6</v>
@@ -2982,7 +2708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>18</v>
       </c>
@@ -3014,7 +2740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>19</v>
       </c>
@@ -3046,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>14</v>
       </c>
@@ -3057,7 +2783,7 @@
         <v>3</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>5</v>
@@ -3068,8 +2794,8 @@
       <c r="G75" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>44</v>
+      <c r="H75" s="2">
+        <v>3</v>
       </c>
       <c r="I75" s="2" t="s">
         <v>6</v>
@@ -3078,7 +2804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>18</v>
       </c>
@@ -3089,7 +2815,7 @@
         <v>14</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>16</v>
@@ -3100,8 +2826,8 @@
       <c r="G76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>108</v>
+      <c r="H76" s="2">
+        <v>0</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>6</v>
@@ -3110,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>22</v>
       </c>
@@ -3132,8 +2858,8 @@
       <c r="G77" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>50</v>
+      <c r="H77" s="2">
+        <v>5</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>9</v>
@@ -3142,7 +2868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>16</v>
       </c>
@@ -3153,7 +2879,7 @@
         <v>14</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>8</v>
@@ -3164,8 +2890,8 @@
       <c r="G78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>51</v>
+      <c r="H78" s="2">
+        <v>8</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>6</v>
@@ -3174,7 +2900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>21</v>
       </c>
@@ -3196,8 +2922,8 @@
       <c r="G79" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H79" s="2" t="s">
-        <v>52</v>
+      <c r="H79" s="2">
+        <v>15</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>6</v>
@@ -3206,7 +2932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>18</v>
       </c>
@@ -3217,7 +2943,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>16</v>
@@ -3228,8 +2954,8 @@
       <c r="G80" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="2" t="s">
-        <v>53</v>
+      <c r="H80" s="2">
+        <v>3</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>6</v>
@@ -3238,7 +2964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>17</v>
       </c>
@@ -3249,7 +2975,7 @@
         <v>3</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>16</v>
@@ -3260,8 +2986,8 @@
       <c r="G81" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="2" t="s">
-        <v>101</v>
+      <c r="H81" s="2">
+        <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>6</v>
@@ -3270,7 +2996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>17</v>
       </c>
@@ -3281,7 +3007,7 @@
         <v>3</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>16</v>
@@ -3292,8 +3018,8 @@
       <c r="G82" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H82" s="2" t="s">
-        <v>54</v>
+      <c r="H82" s="2">
+        <v>10</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>6</v>
@@ -3302,7 +3028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>19</v>
       </c>
@@ -3324,8 +3050,8 @@
       <c r="G83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="2" t="s">
-        <v>55</v>
+      <c r="H83" s="2">
+        <v>2</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>6</v>
@@ -3334,7 +3060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>16</v>
       </c>
@@ -3345,7 +3071,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>16</v>
@@ -3356,8 +3082,8 @@
       <c r="G84" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="2" t="s">
-        <v>19</v>
+      <c r="H84" s="2">
+        <v>3</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>6</v>
@@ -3366,7 +3092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>16</v>
       </c>
@@ -3377,7 +3103,7 @@
         <v>3</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>5</v>
@@ -3388,8 +3114,8 @@
       <c r="G85" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H85" s="2" t="s">
-        <v>56</v>
+      <c r="H85" s="2">
+        <v>4</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>6</v>
@@ -3398,7 +3124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>18</v>
       </c>
@@ -3430,7 +3156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>18</v>
       </c>
@@ -3452,8 +3178,8 @@
       <c r="G87" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H87" s="2" t="s">
-        <v>57</v>
+      <c r="H87" s="2">
+        <v>2</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>11</v>
@@ -3462,7 +3188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>17</v>
       </c>
@@ -3473,7 +3199,7 @@
         <v>14</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>5</v>
@@ -3484,8 +3210,8 @@
       <c r="G88" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H88" s="2" t="s">
-        <v>58</v>
+      <c r="H88" s="2">
+        <v>10</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>6</v>
@@ -3494,7 +3220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>16</v>
       </c>
@@ -3505,7 +3231,7 @@
         <v>3</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>5</v>
@@ -3516,8 +3242,8 @@
       <c r="G89" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H89" s="2" t="s">
-        <v>59</v>
+      <c r="H89" s="2">
+        <v>6</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>6</v>
@@ -3526,7 +3252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>18</v>
       </c>
@@ -3548,8 +3274,8 @@
       <c r="G90" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H90" s="2" t="s">
-        <v>44</v>
+      <c r="H90" s="2">
+        <v>3</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>11</v>
@@ -3558,7 +3284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>17</v>
       </c>
@@ -3569,7 +3295,7 @@
         <v>3</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>16</v>
@@ -3580,8 +3306,8 @@
       <c r="G91" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H91" s="2" t="s">
-        <v>60</v>
+      <c r="H91" s="2">
+        <v>1</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>9</v>
@@ -3590,7 +3316,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>17</v>
       </c>
@@ -3601,7 +3327,7 @@
         <v>3</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>5</v>
@@ -3612,8 +3338,8 @@
       <c r="G92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H92" s="2" t="s">
-        <v>61</v>
+      <c r="H92" s="2">
+        <v>7</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>6</v>
@@ -3622,7 +3348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>18</v>
       </c>
@@ -3633,7 +3359,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>16</v>
@@ -3644,8 +3370,8 @@
       <c r="G93" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H93" s="2" t="s">
-        <v>62</v>
+      <c r="H93" s="2">
+        <v>1</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>6</v>
@@ -3654,7 +3380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>18</v>
       </c>
@@ -3676,8 +3402,8 @@
       <c r="G94" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H94" s="2" t="s">
-        <v>38</v>
+      <c r="H94" s="2">
+        <v>5</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>6</v>
@@ -3686,7 +3412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>18</v>
       </c>
@@ -3697,7 +3423,7 @@
         <v>3</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>5</v>
@@ -3708,8 +3434,8 @@
       <c r="G95" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H95" s="2" t="s">
-        <v>24</v>
+      <c r="H95" s="2">
+        <v>4</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>11</v>
@@ -3718,7 +3444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>17</v>
       </c>
@@ -3729,7 +3455,7 @@
         <v>3</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>5</v>
@@ -3740,8 +3466,8 @@
       <c r="G96" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H96" s="2" t="s">
-        <v>63</v>
+      <c r="H96" s="2">
+        <v>6</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>6</v>
@@ -3750,7 +3476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>15</v>
       </c>
@@ -3761,7 +3487,7 @@
         <v>3</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>18</v>
@@ -3772,8 +3498,8 @@
       <c r="G97" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H97" s="2" t="s">
-        <v>44</v>
+      <c r="H97" s="2">
+        <v>3</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>11</v>
@@ -3782,7 +3508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>19</v>
       </c>
@@ -3814,7 +3540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>16</v>
       </c>
@@ -3825,7 +3551,7 @@
         <v>3</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>18</v>
@@ -3836,8 +3562,8 @@
       <c r="G99" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H99" s="2" t="s">
-        <v>64</v>
+      <c r="H99" s="2">
+        <v>7</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>6</v>
@@ -3846,7 +3572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>19</v>
       </c>
@@ -3868,8 +3594,8 @@
       <c r="G100" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H100" s="2" t="s">
-        <v>65</v>
+      <c r="H100" s="2">
+        <v>2</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>6</v>
@@ -3878,7 +3604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>18</v>
       </c>
@@ -3910,7 +3636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>19</v>
       </c>
@@ -3932,8 +3658,8 @@
       <c r="G102" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H102" s="2" t="s">
-        <v>66</v>
+      <c r="H102" s="2">
+        <v>3</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>11</v>
@@ -3942,7 +3668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>18</v>
       </c>
@@ -3974,7 +3700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>17</v>
       </c>
@@ -3985,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>16</v>
@@ -3996,8 +3722,8 @@
       <c r="G104" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H104" s="2" t="s">
-        <v>67</v>
+      <c r="H104" s="2">
+        <v>10</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>6</v>
@@ -4006,7 +3732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>18</v>
       </c>
@@ -4028,8 +3754,8 @@
       <c r="G105" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H105" s="2" t="s">
-        <v>27</v>
+      <c r="H105" s="2">
+        <v>4</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>9</v>
@@ -4038,7 +3764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>17</v>
       </c>
@@ -4049,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>8</v>
@@ -4070,7 +3796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>19</v>
       </c>
@@ -4102,7 +3828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>17</v>
       </c>
@@ -4134,7 +3860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>17</v>
       </c>
@@ -4145,7 +3871,7 @@
         <v>3</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>16</v>
@@ -4166,7 +3892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>13</v>
       </c>
@@ -4177,7 +3903,7 @@
         <v>14</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>18</v>
@@ -4188,8 +3914,8 @@
       <c r="G110" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H110" s="2" t="s">
-        <v>68</v>
+      <c r="H110" s="2">
+        <v>3</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>6</v>
@@ -4198,7 +3924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>16</v>
       </c>
@@ -4209,7 +3935,7 @@
         <v>14</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>16</v>
@@ -4230,7 +3956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>17</v>
       </c>
@@ -4241,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>16</v>
@@ -4252,8 +3978,8 @@
       <c r="G112" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H112" s="2" t="s">
-        <v>69</v>
+      <c r="H112" s="2">
+        <v>2</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>6</v>
@@ -4262,7 +3988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>17</v>
       </c>
@@ -4273,7 +3999,7 @@
         <v>3</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>18</v>
@@ -4294,7 +4020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>18</v>
       </c>
@@ -4316,8 +4042,8 @@
       <c r="G114" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H114" s="2" t="s">
-        <v>109</v>
+      <c r="H114" s="2">
+        <v>0</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>11</v>
@@ -4326,7 +4052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>16</v>
       </c>
@@ -4337,7 +4063,7 @@
         <v>3</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>16</v>
@@ -4348,8 +4074,8 @@
       <c r="G115" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H115" s="2" t="s">
-        <v>50</v>
+      <c r="H115" s="2">
+        <v>5</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>6</v>
@@ -4358,7 +4084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>18</v>
       </c>
@@ -4380,8 +4106,8 @@
       <c r="G116" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H116" s="2" t="s">
-        <v>70</v>
+      <c r="H116" s="2">
+        <v>1</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>9</v>
@@ -4390,7 +4116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>17</v>
       </c>
@@ -4401,7 +4127,7 @@
         <v>14</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>16</v>
@@ -4412,8 +4138,8 @@
       <c r="G117" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H117" s="2" t="s">
-        <v>71</v>
+      <c r="H117" s="2">
+        <v>3</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>6</v>
@@ -4422,7 +4148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>17</v>
       </c>
@@ -4433,7 +4159,7 @@
         <v>3</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>16</v>
@@ -4454,7 +4180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>18</v>
       </c>
@@ -4465,7 +4191,7 @@
         <v>3</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>16</v>
@@ -4486,7 +4212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>14</v>
       </c>
@@ -4497,7 +4223,7 @@
         <v>3</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>5</v>
@@ -4508,8 +4234,8 @@
       <c r="G120" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H120" s="2" t="s">
-        <v>72</v>
+      <c r="H120" s="2">
+        <v>12</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>6</v>
@@ -4518,7 +4244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>18</v>
       </c>
@@ -4529,7 +4255,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>16</v>
@@ -4540,8 +4266,8 @@
       <c r="G121" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H121" s="2" t="s">
-        <v>69</v>
+      <c r="H121" s="2">
+        <v>2</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>6</v>
@@ -4550,7 +4276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>18</v>
       </c>
@@ -4572,8 +4298,8 @@
       <c r="G122" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H122" s="2" t="s">
-        <v>73</v>
+      <c r="H122" s="2">
+        <v>5</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>11</v>
@@ -4582,7 +4308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>16</v>
       </c>
@@ -4593,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>5</v>
@@ -4604,8 +4330,8 @@
       <c r="G123" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H123" s="2" t="s">
-        <v>74</v>
+      <c r="H123" s="2">
+        <v>4</v>
       </c>
       <c r="I123" s="2" t="s">
         <v>6</v>
@@ -4614,7 +4340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>18</v>
       </c>
@@ -4636,8 +4362,8 @@
       <c r="G124" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H124" s="2" t="s">
-        <v>75</v>
+      <c r="H124" s="2">
+        <v>4</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>9</v>
@@ -4646,7 +4372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>17</v>
       </c>
@@ -4657,7 +4383,7 @@
         <v>3</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>5</v>
@@ -4668,8 +4394,8 @@
       <c r="G125" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H125" s="2" t="s">
-        <v>76</v>
+      <c r="H125" s="2">
+        <v>5</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>6</v>
@@ -4678,7 +4404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>17</v>
       </c>
@@ -4689,7 +4415,7 @@
         <v>3</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>16</v>
@@ -4698,7 +4424,7 @@
         <v>6</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H126">
         <v>6</v>
@@ -4710,7 +4436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>18</v>
       </c>
@@ -4732,8 +4458,8 @@
       <c r="G127" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H127" s="2" t="s">
-        <v>109</v>
+      <c r="H127" s="2">
+        <v>0</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>11</v>
@@ -4742,7 +4468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>18</v>
       </c>
@@ -4764,8 +4490,8 @@
       <c r="G128" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H128" s="2" t="s">
-        <v>44</v>
+      <c r="H128" s="2">
+        <v>3</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>11</v>
@@ -4774,7 +4500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>17</v>
       </c>
@@ -4785,7 +4511,7 @@
         <v>3</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>18</v>
@@ -4796,8 +4522,8 @@
       <c r="G129" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H129" s="2" t="s">
-        <v>77</v>
+      <c r="H129" s="2">
+        <v>2</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>6</v>
@@ -4806,7 +4532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>16</v>
       </c>
@@ -4817,7 +4543,7 @@
         <v>3</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>16</v>
@@ -4828,8 +4554,8 @@
       <c r="G130" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H130" s="2" t="s">
-        <v>78</v>
+      <c r="H130" s="2">
+        <v>4</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>6</v>
@@ -4838,7 +4564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>16</v>
       </c>
@@ -4849,7 +4575,7 @@
         <v>3</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>16</v>
@@ -4860,8 +4586,8 @@
       <c r="G131" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H131" s="2" t="s">
-        <v>79</v>
+      <c r="H131" s="2">
+        <v>1</v>
       </c>
       <c r="I131" s="2" t="s">
         <v>6</v>
@@ -4870,7 +4596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>17</v>
       </c>
@@ -4881,7 +4607,7 @@
         <v>3</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>16</v>
@@ -4892,8 +4618,8 @@
       <c r="G132" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H132" s="2" t="s">
-        <v>69</v>
+      <c r="H132" s="2">
+        <v>2</v>
       </c>
       <c r="I132" s="2" t="s">
         <v>6</v>
@@ -4902,7 +4628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>15</v>
       </c>
@@ -4913,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E133" s="2" t="s">
         <v>16</v>
@@ -4924,8 +4650,8 @@
       <c r="G133" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H133" s="2" t="s">
-        <v>80</v>
+      <c r="H133" s="2">
+        <v>3</v>
       </c>
       <c r="I133" s="2" t="s">
         <v>6</v>
@@ -4934,7 +4660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>18</v>
       </c>
@@ -4956,8 +4682,8 @@
       <c r="G134" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H134" s="2" t="s">
-        <v>81</v>
+      <c r="H134" s="2">
+        <v>2</v>
       </c>
       <c r="I134" s="2" t="s">
         <v>6</v>
@@ -4966,7 +4692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>16</v>
       </c>
@@ -4977,7 +4703,7 @@
         <v>3</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E135" s="2" t="s">
         <v>16</v>
@@ -4998,7 +4724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>15</v>
       </c>
@@ -5009,7 +4735,7 @@
         <v>3</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>16</v>
@@ -5020,8 +4746,8 @@
       <c r="G136" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H136" s="2" t="s">
-        <v>21</v>
+      <c r="H136" s="2">
+        <v>5</v>
       </c>
       <c r="I136" s="2" t="s">
         <v>6</v>
@@ -5030,7 +4756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>18</v>
       </c>
@@ -5050,7 +4776,7 @@
         <v>6</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H137">
         <v>4</v>
@@ -5062,7 +4788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>18</v>
       </c>
@@ -5094,7 +4820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>18</v>
       </c>
@@ -5116,8 +4842,8 @@
       <c r="G139" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H139" s="2" t="s">
-        <v>82</v>
+      <c r="H139" s="2">
+        <v>3</v>
       </c>
       <c r="I139" s="2" t="s">
         <v>11</v>
@@ -5126,7 +4852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>15</v>
       </c>
@@ -5137,7 +4863,7 @@
         <v>3</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>5</v>
@@ -5148,8 +4874,8 @@
       <c r="G140" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H140" s="2" t="s">
-        <v>83</v>
+      <c r="H140" s="2">
+        <v>2</v>
       </c>
       <c r="I140" s="2" t="s">
         <v>6</v>
@@ -5158,7 +4884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>20</v>
       </c>
@@ -5169,7 +4895,7 @@
         <v>3</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>8</v>
@@ -5180,6 +4906,9 @@
       <c r="G141" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H141" s="2">
+        <v>2</v>
+      </c>
       <c r="I141" s="2" t="s">
         <v>11</v>
       </c>
@@ -5187,7 +4916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>21</v>
       </c>
@@ -5219,7 +4948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>17</v>
       </c>
@@ -5230,7 +4959,7 @@
         <v>3</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>16</v>
@@ -5241,8 +4970,8 @@
       <c r="G143" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H143" s="2" t="s">
-        <v>81</v>
+      <c r="H143" s="2">
+        <v>2</v>
       </c>
       <c r="I143" s="2" t="s">
         <v>6</v>
@@ -5251,7 +4980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>17</v>
       </c>
@@ -5262,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>5</v>
@@ -5283,7 +5012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>18</v>
       </c>
@@ -5315,7 +5044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>18</v>
       </c>
@@ -5326,7 +5055,7 @@
         <v>3</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>5</v>
@@ -5337,8 +5066,8 @@
       <c r="G146" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H146" s="2" t="s">
-        <v>84</v>
+      <c r="H146" s="2">
+        <v>5</v>
       </c>
       <c r="I146" s="2" t="s">
         <v>11</v>
@@ -5347,7 +5076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>17</v>
       </c>
@@ -5358,7 +5087,7 @@
         <v>14</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>8</v>
@@ -5369,8 +5098,8 @@
       <c r="G147" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H147" s="2" t="s">
-        <v>85</v>
+      <c r="H147" s="2">
+        <v>8</v>
       </c>
       <c r="I147" s="2" t="s">
         <v>6</v>
@@ -5379,7 +5108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>16</v>
       </c>
@@ -5390,7 +5119,7 @@
         <v>3</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>8</v>
@@ -5401,8 +5130,8 @@
       <c r="G148" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H148" s="2" t="s">
-        <v>20</v>
+      <c r="H148" s="2">
+        <v>6</v>
       </c>
       <c r="I148" s="2" t="s">
         <v>6</v>
@@ -5433,8 +5162,8 @@
       <c r="G149" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H149" s="2" t="s">
-        <v>19</v>
+      <c r="H149" s="2">
+        <v>3</v>
       </c>
       <c r="I149" s="2" t="s">
         <v>6</v>
@@ -5465,8 +5194,8 @@
       <c r="G150" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H150" s="2" t="s">
-        <v>27</v>
+      <c r="H150" s="2">
+        <v>4</v>
       </c>
       <c r="I150" s="2" t="s">
         <v>11</v>
@@ -5497,8 +5226,8 @@
       <c r="G151" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H151" s="2" t="s">
-        <v>86</v>
+      <c r="H151" s="2">
+        <v>5</v>
       </c>
       <c r="I151" s="2" t="s">
         <v>11</v>
@@ -5518,7 +5247,7 @@
         <v>14</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>16</v>
@@ -5529,8 +5258,8 @@
       <c r="G152" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H152" s="2" t="s">
-        <v>87</v>
+      <c r="H152" s="2">
+        <v>5</v>
       </c>
       <c r="I152" s="2" t="s">
         <v>6</v>
@@ -5550,7 +5279,7 @@
         <v>14</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>18</v>
@@ -5561,8 +5290,8 @@
       <c r="G153" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H153" s="2" t="s">
-        <v>88</v>
+      <c r="H153" s="2">
+        <v>2</v>
       </c>
       <c r="I153" s="2" t="s">
         <v>6</v>
@@ -5582,7 +5311,7 @@
         <v>3</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>16</v>
@@ -5593,8 +5322,8 @@
       <c r="G154" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H154" s="2" t="s">
-        <v>89</v>
+      <c r="H154" s="2">
+        <v>3</v>
       </c>
       <c r="I154" s="2" t="s">
         <v>6</v>
@@ -5614,7 +5343,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>8</v>
@@ -5625,8 +5354,8 @@
       <c r="G155" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H155" s="3" t="s">
-        <v>90</v>
+      <c r="H155" s="3">
+        <v>5</v>
       </c>
       <c r="I155" s="2" t="s">
         <v>6</v>
@@ -5646,7 +5375,7 @@
         <v>3</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>16</v>
@@ -5657,8 +5386,8 @@
       <c r="G156" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H156" s="2" t="s">
-        <v>91</v>
+      <c r="H156" s="2">
+        <v>1</v>
       </c>
       <c r="I156" s="2" t="s">
         <v>6</v>
@@ -5689,8 +5418,8 @@
       <c r="G157" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H157" s="2" t="s">
-        <v>92</v>
+      <c r="H157" s="2">
+        <v>5</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>6</v>
@@ -5710,7 +5439,7 @@
         <v>3</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>18</v>
@@ -5753,8 +5482,8 @@
       <c r="G159" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H159" s="2" t="s">
-        <v>93</v>
+      <c r="H159" s="2">
+        <v>8</v>
       </c>
       <c r="I159" s="2" t="s">
         <v>9</v>
@@ -5785,8 +5514,8 @@
       <c r="G160" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H160" s="2" t="s">
-        <v>94</v>
+      <c r="H160" s="2">
+        <v>3</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>11</v>
@@ -5881,8 +5610,8 @@
       <c r="G163" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H163" s="2" t="s">
-        <v>109</v>
+      <c r="H163" s="2">
+        <v>0</v>
       </c>
       <c r="I163" s="2" t="s">
         <v>11</v>
@@ -5902,7 +5631,7 @@
         <v>3</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>5</v>
@@ -5913,8 +5642,8 @@
       <c r="G164" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H164" s="2" t="s">
-        <v>95</v>
+      <c r="H164" s="2">
+        <v>3</v>
       </c>
       <c r="I164" s="2" t="s">
         <v>6</v>
@@ -5945,8 +5674,8 @@
       <c r="G165" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H165" s="2" t="s">
-        <v>96</v>
+      <c r="H165" s="2">
+        <v>2</v>
       </c>
       <c r="I165" s="2" t="s">
         <v>11</v>
@@ -5966,7 +5695,7 @@
         <v>3</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>16</v>
@@ -5977,8 +5706,8 @@
       <c r="G166" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H166" s="2" t="s">
-        <v>114</v>
+      <c r="H166" s="2">
+        <v>5</v>
       </c>
       <c r="I166" s="2" t="s">
         <v>6</v>
@@ -6009,8 +5738,8 @@
       <c r="G167" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H167" s="2" t="s">
-        <v>44</v>
+      <c r="H167" s="2">
+        <v>3</v>
       </c>
       <c r="I167" s="2" t="s">
         <v>11</v>
@@ -6073,8 +5802,8 @@
       <c r="G169" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H169" s="2" t="s">
-        <v>58</v>
+      <c r="H169" s="2">
+        <v>10</v>
       </c>
       <c r="I169" s="2" t="s">
         <v>6</v>
@@ -6094,7 +5823,7 @@
         <v>3</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>8</v>
@@ -6105,8 +5834,8 @@
       <c r="G170" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H170" s="2" t="s">
-        <v>97</v>
+      <c r="H170" s="2">
+        <v>10</v>
       </c>
       <c r="I170" s="2" t="s">
         <v>11</v>
@@ -6126,7 +5855,7 @@
         <v>3</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>16</v>
@@ -6137,8 +5866,8 @@
       <c r="G171" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H171" s="2" t="s">
-        <v>98</v>
+      <c r="H171" s="2">
+        <v>3</v>
       </c>
       <c r="I171" s="2" t="s">
         <v>6</v>
@@ -6158,7 +5887,7 @@
         <v>3</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>5</v>
@@ -6169,8 +5898,8 @@
       <c r="G172" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H172" s="2" t="s">
-        <v>25</v>
+      <c r="H172" s="2">
+        <v>3</v>
       </c>
       <c r="I172" s="2" t="s">
         <v>6</v>
@@ -6190,7 +5919,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>16</v>
@@ -6201,8 +5930,8 @@
       <c r="G173" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H173" s="2" t="s">
-        <v>81</v>
+      <c r="H173" s="2">
+        <v>2</v>
       </c>
       <c r="I173" s="2" t="s">
         <v>6</v>
@@ -6222,7 +5951,7 @@
         <v>3</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>8</v>
@@ -6233,8 +5962,8 @@
       <c r="G174" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H174" s="2" t="s">
-        <v>99</v>
+      <c r="H174" s="2">
+        <v>12</v>
       </c>
       <c r="I174" s="2" t="s">
         <v>6</v>
@@ -6254,7 +5983,7 @@
         <v>14</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E175" s="2" t="s">
         <v>16</v>
@@ -6265,8 +5994,8 @@
       <c r="G175" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H175" s="2" t="s">
-        <v>42</v>
+      <c r="H175" s="2">
+        <v>2</v>
       </c>
       <c r="I175" s="2" t="s">
         <v>6</v>
@@ -6286,7 +6015,7 @@
         <v>3</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E176" s="2" t="s">
         <v>5</v>
@@ -6318,7 +6047,7 @@
         <v>3</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E177" s="2" t="s">
         <v>16</v>
@@ -6329,8 +6058,8 @@
       <c r="G177" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H177" s="2" t="s">
-        <v>79</v>
+      <c r="H177" s="2">
+        <v>1</v>
       </c>
       <c r="I177" s="2" t="s">
         <v>6</v>
@@ -6350,7 +6079,7 @@
         <v>3</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E178" s="2" t="s">
         <v>5</v>
@@ -6361,8 +6090,8 @@
       <c r="G178" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H178" s="2" t="s">
-        <v>21</v>
+      <c r="H178" s="2">
+        <v>5</v>
       </c>
       <c r="I178" s="2" t="s">
         <v>6</v>
@@ -6393,8 +6122,8 @@
       <c r="G179" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H179" s="2" t="s">
-        <v>100</v>
+      <c r="H179" s="2">
+        <v>5</v>
       </c>
       <c r="I179" s="2" t="s">
         <v>11</v>
@@ -6414,7 +6143,7 @@
         <v>3</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E180" s="2" t="s">
         <v>16</v>
@@ -6425,8 +6154,8 @@
       <c r="G180" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H180" s="2" t="s">
-        <v>101</v>
+      <c r="H180" s="2">
+        <v>1</v>
       </c>
       <c r="I180" s="2" t="s">
         <v>6</v>
@@ -6446,7 +6175,7 @@
         <v>3</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E181" s="2" t="s">
         <v>16</v>
@@ -6478,7 +6207,7 @@
         <v>3</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>18</v>
@@ -6489,8 +6218,8 @@
       <c r="G182" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H182" s="2" t="s">
-        <v>113</v>
+      <c r="H182" s="2">
+        <v>2</v>
       </c>
       <c r="I182" s="2" t="s">
         <v>6</v>
@@ -6521,8 +6250,8 @@
       <c r="G183" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H183" s="2" t="s">
-        <v>102</v>
+      <c r="H183" s="2">
+        <v>3</v>
       </c>
       <c r="I183" s="2" t="s">
         <v>11</v>
@@ -6542,7 +6271,7 @@
         <v>14</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E184" s="2" t="s">
         <v>5</v>
@@ -6553,8 +6282,8 @@
       <c r="G184" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H184" s="2" t="s">
-        <v>103</v>
+      <c r="H184" s="2">
+        <v>6</v>
       </c>
       <c r="I184" s="2" t="s">
         <v>9</v>
@@ -6574,7 +6303,7 @@
         <v>3</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E185" s="2" t="s">
         <v>5</v>
@@ -6585,8 +6314,8 @@
       <c r="G185" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H185" s="2" t="s">
-        <v>104</v>
+      <c r="H185" s="2">
+        <v>4</v>
       </c>
       <c r="I185" s="2" t="s">
         <v>6</v>
@@ -6606,7 +6335,7 @@
         <v>3</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>16</v>
@@ -6617,8 +6346,8 @@
       <c r="G186" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H186" s="2" t="s">
-        <v>105</v>
+      <c r="H186" s="2">
+        <v>2</v>
       </c>
       <c r="I186" s="2" t="s">
         <v>6</v>
@@ -6638,7 +6367,7 @@
         <v>3</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E187" s="2" t="s">
         <v>5</v>
@@ -6649,8 +6378,8 @@
       <c r="G187" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H187" s="2" t="s">
-        <v>24</v>
+      <c r="H187" s="2">
+        <v>4</v>
       </c>
       <c r="I187" s="2" t="s">
         <v>6</v>
@@ -6670,7 +6399,7 @@
         <v>14</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E188" s="2" t="s">
         <v>16</v>
@@ -6681,8 +6410,8 @@
       <c r="G188" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H188" s="2" t="s">
-        <v>112</v>
+      <c r="H188" s="2">
+        <v>8</v>
       </c>
       <c r="I188" s="2" t="s">
         <v>6</v>
@@ -6713,8 +6442,8 @@
       <c r="G189" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H189" s="2" t="s">
-        <v>106</v>
+      <c r="H189" s="2">
+        <v>7</v>
       </c>
       <c r="I189" s="2" t="s">
         <v>6</v>
@@ -6745,8 +6474,8 @@
       <c r="G190" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H190" s="2" t="s">
-        <v>111</v>
+      <c r="H190" s="2">
+        <v>7</v>
       </c>
       <c r="I190" s="2" t="s">
         <v>6</v>
@@ -6766,7 +6495,7 @@
         <v>3</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E191" s="2" t="s">
         <v>5</v>
@@ -6777,8 +6506,8 @@
       <c r="G191" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H191" s="3" t="s">
-        <v>107</v>
+      <c r="H191" s="3">
+        <v>4</v>
       </c>
       <c r="I191" s="2" t="s">
         <v>6</v>
@@ -6798,7 +6527,7 @@
         <v>3</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E192" s="2" t="s">
         <v>18</v>
@@ -6809,8 +6538,8 @@
       <c r="G192" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H192" s="2" t="s">
-        <v>101</v>
+      <c r="H192" s="2">
+        <v>1</v>
       </c>
       <c r="I192" s="2" t="s">
         <v>6</v>
@@ -6839,10 +6568,10 @@
         <v>6</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H193" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="H193" s="2">
+        <v>1</v>
       </c>
       <c r="I193" s="2" t="s">
         <v>11</v>
@@ -6862,7 +6591,7 @@
         <v>3</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>18</v>
@@ -6873,8 +6602,8 @@
       <c r="G194" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H194" s="2" t="s">
-        <v>109</v>
+      <c r="H194" s="2">
+        <v>0</v>
       </c>
       <c r="I194" s="2" t="s">
         <v>6</v>
@@ -6882,9 +6611,266 @@
       <c r="J194" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="195" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H195" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A4B97804575CB7449BE290F2DFA70D34" ma:contentTypeVersion="10" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="110ef2db02b79dec7a90c3bc666c7eae">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6a531a1-fad5-4186-b0d8-4d69beb33d58" xmlns:ns3="271c1a74-9ad3-4c6d-8b16-3dcd57ae220e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="831551c7490b90c7bd397af23fe4945b" ns2:_="" ns3:_="">
+    <xsd:import namespace="f6a531a1-fad5-4186-b0d8-4d69beb33d58"/>
+    <xsd:import namespace="271c1a74-9ad3-4c6d-8b16-3dcd57ae220e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f6a531a1-fad5-4186-b0d8-4d69beb33d58" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="271c1a74-9ad3-4c6d-8b16-3dcd57ae220e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EAA28BE-699E-451A-BE50-80AEC388C3D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6a531a1-fad5-4186-b0d8-4d69beb33d58"/>
+    <ds:schemaRef ds:uri="271c1a74-9ad3-4c6d-8b16-3dcd57ae220e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAA9737C-AA70-451B-9318-8FDD54F4F172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B868EF-4D17-425C-A277-302DADAC6122}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>